<commit_message>
figure  TG [M+Na]+ corrections. Fix bug problems with the control in [M+Na]+ and [M+H]+
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/01-FA_Whitelist_PL.xlsx
+++ b/ConfigurationFiles/01-FA_Whitelist_PL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -75,21 +75,9 @@
     <t>P-20:0</t>
   </si>
   <si>
-    <t>sn1</t>
-  </si>
-  <si>
-    <t>sn2</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
-    <t>sn3</t>
-  </si>
-  <si>
-    <t>sn4</t>
-  </si>
-  <si>
     <t>PL</t>
   </si>
   <si>
@@ -100,6 +88,18 @@
   </si>
   <si>
     <t>FA16:1</t>
+  </si>
+  <si>
+    <t>fa1</t>
+  </si>
+  <si>
+    <t>fa2</t>
+  </si>
+  <si>
+    <t>fa3</t>
+  </si>
+  <si>
+    <t>fa4</t>
   </si>
 </sst>
 </file>
@@ -115,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +427,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,39 +440,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -473,36 +480,36 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -510,19 +517,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -530,19 +537,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -550,19 +557,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -570,16 +577,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -587,16 +594,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,16 +611,16 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -621,16 +628,16 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -638,16 +645,16 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -655,16 +662,16 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,16 +679,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -689,10 +696,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -700,10 +707,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -711,10 +718,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -722,10 +729,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,10 +740,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -744,10 +751,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>